<commit_message>
stuck on ts showing up
</commit_message>
<xml_diff>
--- a/code/paleo_flow/data/sites_monthly.xlsx
+++ b/code/paleo_flow/data/sites_monthly.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stagge.11\Documents\Dropbox\work_folder\projects_research\code\paleo_flow_shiny\code\paleo_flow\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1245" yWindow="900" windowWidth="19035" windowHeight="5400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sites_monthly" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -120,8 +125,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -157,6 +162,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -203,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -235,9 +248,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,6 +283,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -444,14 +459,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" customWidth="1"/>
@@ -465,7 +480,7 @@
     <col min="10" max="1023" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,53 +518,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2">
-        <v>40.965277999999998</v>
-      </c>
-      <c r="L2">
-        <v>-110.852778</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -561,33 +538,33 @@
         <v>31</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
       </c>
-      <c r="I3" t="s">
-        <v>16</v>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K3">
-        <v>41.744444000000001</v>
+        <v>40.965277999999998</v>
       </c>
       <c r="L3">
-        <v>-111.78361099999999</v>
+        <v>-110.852778</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -599,27 +576,65 @@
         <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
       <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4">
+        <v>41.744444000000001</v>
+      </c>
+      <c r="L4">
+        <v>-111.78361099999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" t="s">
         <v>19</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J5" t="s">
         <v>27</v>
       </c>
-      <c r="K4">
+      <c r="K5">
         <v>40.737222000000003</v>
       </c>
-      <c r="L4">
+      <c r="L5">
         <v>-111.24722199999999</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1"/>
+    <hyperlink ref="I5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Fixed processing issue with flows
</commit_message>
<xml_diff>
--- a/code/paleo_flow/data/sites_monthly.xlsx
+++ b/code/paleo_flow/data/sites_monthly.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+  <si>
+    <t xml:space="preserve">orig_order</t>
+  </si>
   <si>
     <t xml:space="preserve">site_group</t>
   </si>
@@ -56,6 +59,36 @@
   </si>
   <si>
     <t xml:space="preserve">lon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adjustment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reported_cal_r2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reported_val_re</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reported_cal_see</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reported_val_rmse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reported_val_press</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reported_units</t>
+  </si>
+  <si>
+    <t xml:space="preserve">val_method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
   </si>
   <si>
     <t xml:space="preserve">USA, UT</t>
@@ -227,27 +260,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1048576"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="52.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="144.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="34.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="62.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="52.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="50.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="144.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="34.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="62.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.68"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -284,125 +317,166 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>12</v>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="0" t="n">
         <v>40.965278</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="M2" s="0" t="n">
         <v>-110.852778</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>41.744444</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>-111.783611</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="0" t="s">
+      <c r="C4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K3" s="0" t="n">
-        <v>41.744444</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>-111.783611</v>
+      <c r="F4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>40.737222</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>-111.247222</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="K4" s="0" t="n">
-        <v>40.737222</v>
-      </c>
-      <c r="L4" s="0" t="n">
-        <v>-111.247222</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1" display="https://waterdata.usgs.gov/nwis/uv?site_no=10128500"/>
+    <hyperlink ref="J4" r:id="rId1" display="https://waterdata.usgs.gov/nwis/uv?site_no=10128500"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>